<commit_message>
fixed description for elapsed time
</commit_message>
<xml_diff>
--- a/dist/cosasreports.xlsx
+++ b/dist/cosasreports.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="243">
   <si>
     <t>cosasreports</t>
   </si>
@@ -186,37 +186,40 @@
     <t>The time when an event has ceased.</t>
   </si>
   <si>
+    <t>The interval between two reference points in time. (in seconds)</t>
+  </si>
+  <si>
+    <t>Number of rows added to a database table</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_subjects</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_clinical</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_samples</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_samplePreparation</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_sequencing</t>
+  </si>
+  <si>
+    <t>Number of rows added to umdm_files</t>
+  </si>
+  <si>
+    <t>A specific stage of progression through a sequential process.</t>
+  </si>
+  <si>
+    <t>A written explanation, observation or criticism added to textual material.</t>
+  </si>
+  <si>
+    <t>A database table is a set of named columns with zero or more rows composed of cells that contain column values and is part of a database.</t>
+  </si>
+  <si>
     <t>The interval between two reference points in time. (in milliseconds)</t>
-  </si>
-  <si>
-    <t>Number of rows added to a database table</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_subjects</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_clinical</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_samples</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_samplePreparation</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_sequencing</t>
-  </si>
-  <si>
-    <t>Number of rows added to umdm_files</t>
-  </si>
-  <si>
-    <t>A specific stage of progression through a sequential process.</t>
-  </si>
-  <si>
-    <t>A written explanation, observation or criticism added to textual material.</t>
-  </si>
-  <si>
-    <t>A database table is a set of named columns with zero or more rows composed of cells that contain column values and is part of a database.</t>
   </si>
   <si>
     <t>The information contained in a data field. It may represent a numeric quantity, a textual characterization, a date or time measurement, or some other state, depending on the nature of the attribute.</t>
@@ -1115,16 +1118,16 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1173,25 +1176,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1298,7 +1301,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>27</v>
@@ -1307,31 +1310,31 @@
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1345,10 +1348,10 @@
         <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1374,10 +1377,10 @@
         <v>50</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1403,10 +1406,10 @@
         <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1432,7 +1435,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -1461,10 +1464,10 @@
         <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1490,10 +1493,10 @@
         <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1519,10 +1522,10 @@
         <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1548,7 +1551,7 @@
         <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1577,10 +1580,10 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1609,10 +1612,10 @@
         <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1641,10 +1644,10 @@
         <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1673,10 +1676,10 @@
         <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1705,10 +1708,10 @@
         <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1737,10 +1740,10 @@
         <v>62</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1769,10 +1772,10 @@
         <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1801,10 +1804,10 @@
         <v>64</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1830,10 +1833,10 @@
         <v>49</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1859,10 +1862,10 @@
         <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1888,10 +1891,10 @@
         <v>63</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1906,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1920,10 +1923,10 @@
         <v>65</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1949,7 +1952,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -1978,10 +1981,10 @@
         <v>53</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2007,10 +2010,10 @@
         <v>54</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -2033,13 +2036,13 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2068,7 +2071,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -2083,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2097,10 +2100,10 @@
         <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2123,13 +2126,13 @@
         <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2152,13 +2155,13 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -2181,13 +2184,13 @@
         <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -2210,13 +2213,13 @@
         <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -2239,13 +2242,13 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -2310,39 +2313,39 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2350,159 +2353,159 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2510,39 +2513,39 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2550,19 +2553,19 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2570,79 +2573,79 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2650,79 +2653,79 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2730,39 +2733,39 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2863,231 +2866,231 @@
         <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D2">
         <v>3436</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D3">
         <v>3283</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D6">
         <v>2422</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D7">
         <v>2421</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D8">
         <v>3431</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D9">
         <v>3096</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11">
         <v>3695</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D12">
         <v>3357</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D13">
         <v>221</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -3095,138 +3098,138 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D15">
         <v>1812</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D16">
         <v>214</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D17">
         <v>148</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D18">
         <v>3081</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D19">
         <v>153</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D20">
         <v>3802</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21">
         <v>3359</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D22">
         <v>3080</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3284,121 +3287,121 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new report entity
</commit_message>
<xml_diff>
--- a/dist/cosasreports.xlsx
+++ b/dist/cosasreports.xlsx
@@ -13,13 +13,14 @@
     <sheet name="tags" sheetId="4" r:id="rId4"/>
     <sheet name="cosasreports_refs_datahandling" sheetId="5" r:id="rId5"/>
     <sheet name="cosasreports_refs_status" sheetId="6" r:id="rId6"/>
+    <sheet name="cosasreports_refs_keytypes" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="289">
   <si>
     <t>cosasreports</t>
   </si>
@@ -33,7 +34,7 @@
     <t>Reference Tables</t>
   </si>
   <si>
-    <t>Reports on COSAS jobs, imports, and processing (v1.2.0, 2022-03-02)</t>
+    <t>Reports on COSAS jobs, imports, and processing (v1.4.0, 2022-04-19)</t>
   </si>
   <si>
     <t>Reference tables for COSAS Reports</t>
@@ -48,6 +49,9 @@
     <t>processingsteps</t>
   </si>
   <si>
+    <t>attributesummary</t>
+  </si>
+  <si>
     <t>template</t>
   </si>
   <si>
@@ -57,30 +61,45 @@
     <t>status</t>
   </si>
   <si>
+    <t>keytypes</t>
+  </si>
+  <si>
     <t>COSAS Daily Imports</t>
   </si>
   <si>
     <t>COSAS Processing Steps</t>
   </si>
   <si>
+    <t>COSAS Attribute Summary</t>
+  </si>
+  <si>
     <t>Historical records of daily COSAS imports</t>
   </si>
   <si>
     <t>Historical records of steps involved in the processing of daily cosas jobs</t>
   </si>
   <si>
+    <t>Summary of attributes used by COSAS table and the percentage of available data</t>
+  </si>
+  <si>
     <t>Basic (non-analytical) operations of some data, either a file or equivalent entity in memory, such that the same basic type of data is consumed as input and generated as output.</t>
   </si>
   <si>
     <t>A condition or state at a particular time.</t>
   </si>
   <si>
+    <t>A database key is an informational entity whose value is constructed from one or more database columns.</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C73599</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C45279</t>
   </si>
   <si>
+    <t>http://purl.allotrope.org/ontologies/result#AFR_0001213</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
   </si>
   <si>
@@ -90,6 +109,9 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
   </si>
   <si>
+    <t>http://semanticscience.org/resource/SIO_000762</t>
+  </si>
+  <si>
     <t>cosasreports_refs_template</t>
   </si>
   <si>
@@ -99,6 +121,9 @@
     <t>cosasreports_processingsteps</t>
   </si>
   <si>
+    <t>cosasreports_attributesummary</t>
+  </si>
+  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -153,6 +178,27 @@
     <t>databaseTable</t>
   </si>
   <si>
+    <t>dateLastUpdated</t>
+  </si>
+  <si>
+    <t>databaseColumn</t>
+  </si>
+  <si>
+    <t>databaseKey</t>
+  </si>
+  <si>
+    <t>countOfValues</t>
+  </si>
+  <si>
+    <t>totalValues</t>
+  </si>
+  <si>
+    <t>differenceInValues</t>
+  </si>
+  <si>
+    <t>percentComplete</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -222,6 +268,24 @@
     <t>The interval between two reference points in time. (in milliseconds)</t>
   </si>
   <si>
+    <t>A data item that indicates the time when data about the sample collection was last updated in a database.</t>
+  </si>
+  <si>
+    <t>A database collumn is a column in a database table.</t>
+  </si>
+  <si>
+    <t>Determining the number or amount of something.</t>
+  </si>
+  <si>
+    <t>Pertaining to an entirety or whole, also constituting the full quantity or extent; complete; derived by addition.</t>
+  </si>
+  <si>
+    <t>The quality of being unlike or dissimilar.</t>
+  </si>
+  <si>
+    <t>A fraction or ratio with 100 understood as the denominator.</t>
+  </si>
+  <si>
     <t>The information contained in a data field. It may represent a numeric quantity, a textual characterization, a date or time measurement, or some other state, depending on the nature of the attribute.</t>
   </si>
   <si>
@@ -270,6 +334,21 @@
     <t>http://semanticscience.org/resource/SIO_000754</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/OBIB_0000681</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000757</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25304</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C46003</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25613</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
   </si>
   <si>
@@ -321,6 +400,9 @@
     <t>cosasreports_refs_status</t>
   </si>
   <si>
+    <t>cosasreports_refs_keytypes</t>
+  </si>
+  <si>
     <t>label</t>
   </si>
   <si>
@@ -372,6 +454,9 @@
     <t>operation:2409</t>
   </si>
   <si>
+    <t>AFR:0001213</t>
+  </si>
+  <si>
     <t>NCIT:C165071</t>
   </si>
   <si>
@@ -381,6 +466,9 @@
     <t>NCIT:C25164</t>
   </si>
   <si>
+    <t>NCIT:C25304</t>
+  </si>
+  <si>
     <t>NCIT:C25364</t>
   </si>
   <si>
@@ -393,6 +481,9 @@
     <t>NCIT:C25463</t>
   </si>
   <si>
+    <t>NCIT:C25613</t>
+  </si>
+  <si>
     <t>NCIT:C25688</t>
   </si>
   <si>
@@ -405,6 +496,9 @@
     <t>NCIT:C45677</t>
   </si>
   <si>
+    <t>NCIT:C46003</t>
+  </si>
+  <si>
     <t>NCIT:C48176</t>
   </si>
   <si>
@@ -429,18 +523,33 @@
     <t>NCIT:C82964</t>
   </si>
   <si>
+    <t>OBIB:0000681</t>
+  </si>
+  <si>
     <t>SIO:000754</t>
   </si>
   <si>
+    <t>SIO:000757</t>
+  </si>
+  <si>
+    <t>SIO:000762</t>
+  </si>
+  <si>
     <t>EDAM</t>
   </si>
   <si>
     <t>operation</t>
   </si>
   <si>
+    <t>AFR</t>
+  </si>
+  <si>
     <t>NCIT</t>
   </si>
   <si>
+    <t>OBIB</t>
+  </si>
+  <si>
     <t>SIO</t>
   </si>
   <si>
@@ -760,6 +869,24 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C47896</t>
+  </si>
+  <si>
+    <t>foreign database key</t>
+  </si>
+  <si>
+    <t>primary database key</t>
+  </si>
+  <si>
+    <t>A foreign database key is a database key that refers to a key in some table.</t>
+  </si>
+  <si>
+    <t>A primary database key is a database key that identifies every row of a table.</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000764</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000763</t>
   </si>
 </sst>
 </file>
@@ -1127,19 +1254,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1180,7 +1307,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1188,25 +1315,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1217,13 +1344,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1234,27 +1361,30 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1264,14 +1394,11 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1282,22 +1409,58 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="s">
-        <v>23</v>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId3" location="AFR_0001213"/>
     <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1305,7 +1468,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1313,57 +1476,57 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1380,19 +1543,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1409,19 +1572,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1438,19 +1601,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1467,19 +1630,19 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1496,19 +1659,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1525,19 +1688,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1554,16 +1717,16 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1583,19 +1746,19 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1610,24 +1773,24 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1642,24 +1805,24 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1674,24 +1837,24 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1706,24 +1869,24 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1738,24 +1901,24 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1770,24 +1933,24 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1802,24 +1965,24 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1836,19 +1999,19 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -1865,19 +2028,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1894,19 +2057,19 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1923,19 +2086,19 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1950,24 +2113,24 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1984,19 +2147,19 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2013,19 +2176,19 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -2042,19 +2205,19 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2071,19 +2234,19 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -2098,24 +2261,24 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2132,19 +2295,19 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2153,27 +2316,27 @@
         <v>0</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -2190,19 +2353,19 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -2219,19 +2382,19 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -2248,30 +2411,294 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" t="s">
         <v>87</v>
       </c>
-      <c r="E32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="b">
+      <c r="D36" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2307,6 +2734,15 @@
     <hyperlink ref="D30" r:id="rId28"/>
     <hyperlink ref="D31" r:id="rId29"/>
     <hyperlink ref="D32" r:id="rId30"/>
+    <hyperlink ref="D33" r:id="rId31"/>
+    <hyperlink ref="D34" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D36" r:id="rId34"/>
+    <hyperlink ref="D37" r:id="rId35"/>
+    <hyperlink ref="D38" r:id="rId36"/>
+    <hyperlink ref="D39" r:id="rId37"/>
+    <hyperlink ref="D40" r:id="rId38"/>
+    <hyperlink ref="D41" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2314,7 +2750,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2322,462 +2758,602 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E13" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E21" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>142</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" t="s">
+        <v>177</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E28" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2788,8 +3364,8 @@
     <hyperlink ref="A3" r:id="rId4"/>
     <hyperlink ref="C3" r:id="rId5"/>
     <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
+    <hyperlink ref="A4" r:id="rId7" location="AFR_0001213"/>
+    <hyperlink ref="C4" r:id="rId8" location="AFR_0001213"/>
     <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
     <hyperlink ref="A5" r:id="rId10"/>
     <hyperlink ref="C5" r:id="rId11"/>
@@ -2848,6 +3424,27 @@
     <hyperlink ref="A23" r:id="rId64"/>
     <hyperlink ref="C23" r:id="rId65"/>
     <hyperlink ref="F23" r:id="rId66" location="isAssociatedWith"/>
+    <hyperlink ref="A24" r:id="rId67"/>
+    <hyperlink ref="C24" r:id="rId68"/>
+    <hyperlink ref="F24" r:id="rId69" location="isAssociatedWith"/>
+    <hyperlink ref="A25" r:id="rId70"/>
+    <hyperlink ref="C25" r:id="rId71"/>
+    <hyperlink ref="F25" r:id="rId72" location="isAssociatedWith"/>
+    <hyperlink ref="A26" r:id="rId73"/>
+    <hyperlink ref="C26" r:id="rId74"/>
+    <hyperlink ref="F26" r:id="rId75" location="isAssociatedWith"/>
+    <hyperlink ref="A27" r:id="rId76"/>
+    <hyperlink ref="C27" r:id="rId77"/>
+    <hyperlink ref="F27" r:id="rId78" location="isAssociatedWith"/>
+    <hyperlink ref="A28" r:id="rId79"/>
+    <hyperlink ref="C28" r:id="rId80"/>
+    <hyperlink ref="F28" r:id="rId81" location="isAssociatedWith"/>
+    <hyperlink ref="A29" r:id="rId82"/>
+    <hyperlink ref="C29" r:id="rId83"/>
+    <hyperlink ref="F29" r:id="rId84" location="isAssociatedWith"/>
+    <hyperlink ref="A30" r:id="rId85"/>
+    <hyperlink ref="C30" r:id="rId86"/>
+    <hyperlink ref="F30" r:id="rId87" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2863,410 +3460,410 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D2">
         <v>3436</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
         <v>171</v>
-      </c>
-      <c r="C3" t="s">
-        <v>137</v>
       </c>
       <c r="D3">
         <v>3283</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D6">
         <v>2422</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D7">
         <v>2421</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>202</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D8">
         <v>3431</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D9">
         <v>3096</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D11">
         <v>3695</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D12">
         <v>3357</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>207</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D13">
         <v>222</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D14">
         <v>221</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D16">
         <v>1812</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D17">
         <v>214</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D18">
         <v>148</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D19">
         <v>3081</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D20">
         <v>153</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D21">
         <v>3802</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D22">
         <v>3359</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D23">
         <v>3080</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D24">
         <v>2428</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3309,138 +3906,138 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>240</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>242</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>244</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3455,4 +4052,72 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3">
+        <v>499</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added displayName to mappings
</commit_message>
<xml_diff>
--- a/dist/cosasreports.xlsx
+++ b/dist/cosasreports.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="299">
   <si>
     <t>cosasreports</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Reference Tables</t>
   </si>
   <si>
-    <t>Reports on COSAS jobs, imports, and processing (v1.5.0, 2022-06-29)</t>
+    <t>Reports on COSAS jobs, imports, and processing (v1.6.0, 2022-07-29)</t>
   </si>
   <si>
     <t>Reference tables for COSAS Reports</t>
@@ -187,6 +187,9 @@
     <t>databaseColumn</t>
   </si>
   <si>
+    <t>displayName</t>
+  </si>
+  <si>
     <t>databaseKey</t>
   </si>
   <si>
@@ -280,6 +283,9 @@
     <t>A database collumn is a column in a database table.</t>
   </si>
   <si>
+    <t>The standardized text associated with a code in a particular code system.</t>
+  </si>
+  <si>
     <t>Determining the number or amount of something.</t>
   </si>
   <si>
@@ -349,6 +355,9 @@
     <t>SIO_000757</t>
   </si>
   <si>
+    <t>NCIT_C70896</t>
+  </si>
+  <si>
     <t>NCIT_C25304</t>
   </si>
   <si>
@@ -512,6 +521,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C73599</t>
@@ -1275,16 +1287,16 @@
         <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1330,25 +1342,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1474,7 +1486,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1482,40 +1494,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1526,13 +1538,13 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1555,13 +1567,13 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1584,13 +1596,13 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1613,13 +1625,13 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1642,10 +1654,10 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E6" t="s">
         <v>38</v>
@@ -1671,13 +1683,13 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1700,13 +1712,13 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1729,13 +1741,13 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1758,10 +1770,10 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1787,13 +1799,13 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1819,13 +1831,13 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1851,13 +1863,13 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1883,13 +1895,13 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1915,13 +1927,13 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1947,13 +1959,13 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1979,13 +1991,13 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -2011,13 +2023,13 @@
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -2040,13 +2052,13 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -2069,10 +2081,10 @@
         <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
         <v>38</v>
@@ -2098,13 +2110,13 @@
         <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -2127,13 +2139,13 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -2148,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2159,13 +2171,13 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2188,13 +2200,13 @@
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -2217,13 +2229,13 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2246,13 +2258,13 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -2281,7 +2293,7 @@
         <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2296,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2307,13 +2319,13 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -2336,13 +2348,13 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -2365,10 +2377,10 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
         <v>38</v>
@@ -2394,13 +2406,13 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -2423,13 +2435,13 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -2452,13 +2464,13 @@
         <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -2471,9 +2483,6 @@
       </c>
       <c r="I33" t="b">
         <v>0</v>
-      </c>
-      <c r="L33" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2484,13 +2493,13 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -2503,6 +2512,9 @@
       </c>
       <c r="I34" t="b">
         <v>0</v>
+      </c>
+      <c r="L34" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2513,13 +2525,13 @@
         <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -2542,13 +2554,13 @@
         <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2571,13 +2583,13 @@
         <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2594,31 +2606,31 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E38" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2629,25 +2641,25 @@
         <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2658,13 +2670,13 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2687,13 +2699,13 @@
         <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D41" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2716,13 +2728,13 @@
         <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2734,6 +2746,35 @@
         <v>0</v>
       </c>
       <c r="I42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2744,7 +2785,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2755,19 +2796,19 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2778,196 +2819,196 @@
         <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E11" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2978,36 +3019,36 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E12" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3018,16 +3059,16 @@
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E14" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3038,136 +3079,136 @@
         <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3178,116 +3219,116 @@
         <v>102</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E22" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E25" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E26" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E27" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3298,76 +3339,96 @@
         <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E28" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E29" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E30" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" t="s">
-        <v>181</v>
-      </c>
-      <c r="E31" t="s">
-        <v>182</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>183</v>
+      <c r="C32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3432,6 +3493,8 @@
     <hyperlink ref="F30" r:id="rId58" location="isAssociatedWith"/>
     <hyperlink ref="C31" r:id="rId59"/>
     <hyperlink ref="F31" r:id="rId60" location="isAssociatedWith"/>
+    <hyperlink ref="C32" r:id="rId61"/>
+    <hyperlink ref="F32" r:id="rId62" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3447,410 +3510,410 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D2">
         <v>3436</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D3">
         <v>3283</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D6">
         <v>2422</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D7">
         <v>2421</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D8">
         <v>3431</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D9">
         <v>3096</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D11">
         <v>3695</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D12">
         <v>3357</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C13" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D13">
         <v>222</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D14">
         <v>221</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B15" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D16">
         <v>1812</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C17" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D17">
         <v>214</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D18">
         <v>148</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C19" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D19">
         <v>3081</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D20">
         <v>153</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C21" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D21">
         <v>3802</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C22" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D22">
         <v>3359</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D23">
         <v>3080</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C24" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D24">
         <v>2428</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3893,138 +3956,138 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D8" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -4051,53 +4114,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D2">
         <v>500</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D3">
         <v>499</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
init jobs emx and script
</commit_message>
<xml_diff>
--- a/dist/cosasreports.xlsx
+++ b/dist/cosasreports.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="319">
   <si>
     <t>cosasreports</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Reference Tables</t>
   </si>
   <si>
-    <t>Reports on COSAS jobs, imports, and processing (v1.7.0, 2023-07-05)</t>
+    <t>Reports on COSAS jobs, imports, and processing (v1.8.0, 2023-07-14)</t>
   </si>
   <si>
     <t>Reference tables for COSAS Reports</t>
@@ -55,6 +55,9 @@
     <t>datasources</t>
   </si>
   <si>
+    <t>jobs</t>
+  </si>
+  <si>
     <t>template</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
     <t>Overview on the data sources connected to COSAS</t>
   </si>
   <si>
+    <t>Overview on scheduled jobs</t>
+  </si>
+  <si>
     <t>Basic (non-analytical) operations of some data, either a file or equivalent entity in memory, such that the same basic type of data is consumed as input and generated as output.</t>
   </si>
   <si>
@@ -136,6 +142,9 @@
     <t>cosasreports_datasources</t>
   </si>
   <si>
+    <t>cosasreports_jobs</t>
+  </si>
+  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -226,12 +235,21 @@
     <t>metadata</t>
   </si>
   <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>cron</t>
+  </si>
+  <si>
+    <t>dateLastRun</t>
+  </si>
+  <si>
+    <t>isStable</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>codesystem</t>
   </si>
   <si>
@@ -514,96 +532,96 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C82964</t>
   </si>
   <si>
+    <t>http://edamontology.org/operation_2409</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45279</t>
+  </si>
+  <si>
+    <t>http://purl.allotrope.org/ontologies/result#AFR_0001213</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25688</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45279</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/operation_2409</t>
-  </si>
-  <si>
-    <t>http://purl.allotrope.org/ontologies/result#AFR_0001213</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C73599</t>
   </si>
   <si>
     <t>http://semanticscience.org/resource/SIO_000762</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C73599</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25463</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000757</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000034</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C82573</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C82572</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25304</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C78441</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C46003</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000754</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBIB_0000681</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_1056</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C48176</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25304</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C46003</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C78441</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25613</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25463</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C82573</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000754</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_1056</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000034</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000757</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBIB_0000681</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C82572</t>
-  </si>
-  <si>
     <t>NCIT</t>
   </si>
   <si>
@@ -616,10 +634,10 @@
     <t>SIO</t>
   </si>
   <si>
+    <t>OBIB</t>
+  </si>
+  <si>
     <t>data</t>
-  </si>
-  <si>
-    <t>OBIB</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -1326,19 +1344,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1376,7 +1394,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1384,25 +1402,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1413,13 +1431,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1430,13 +1448,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1447,13 +1465,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1464,24 +1482,21 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
+      <c r="D6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1491,14 +1506,11 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1509,13 +1521,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1526,13 +1538,30 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1571,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1550,60 +1579,60 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1620,19 +1649,19 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1649,19 +1678,19 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1678,19 +1707,19 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1707,19 +1736,19 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1736,19 +1765,19 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1765,19 +1794,19 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1794,19 +1823,19 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1823,16 +1852,16 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1852,19 +1881,19 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1879,24 +1908,24 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1911,56 +1940,56 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>136</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1975,24 +2004,24 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -2007,24 +2036,24 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -2039,24 +2068,24 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -2071,24 +2100,24 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -2105,19 +2134,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -2134,19 +2163,19 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -2163,19 +2192,19 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -2192,19 +2221,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -2219,24 +2248,24 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2253,19 +2282,19 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -2282,19 +2311,19 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2311,19 +2340,19 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -2340,19 +2369,19 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2367,24 +2396,24 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -2401,19 +2430,19 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -2430,19 +2459,19 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -2459,19 +2488,19 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -2488,19 +2517,19 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -2517,19 +2546,19 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -2546,19 +2575,19 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -2573,24 +2602,24 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -2607,19 +2636,19 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2636,19 +2665,19 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2665,19 +2694,19 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -2694,16 +2723,16 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -2720,16 +2749,16 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2744,21 +2773,21 @@
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2775,16 +2804,16 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2801,19 +2830,13 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" t="s">
-        <v>103</v>
-      </c>
-      <c r="D43" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -2822,27 +2845,21 @@
         <v>0</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -2859,19 +2876,13 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -2888,19 +2899,13 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="E46" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -2917,19 +2922,13 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" t="s">
-        <v>107</v>
-      </c>
-      <c r="D47" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -2941,6 +2940,151 @@
         <v>0</v>
       </c>
       <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2959,22 +3103,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2985,36 +3129,36 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3025,36 +3169,36 @@
         <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3065,156 +3209,156 @@
         <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E9" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E10" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E11" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E12" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3225,216 +3369,216 @@
         <v>124</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D17" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E17" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E18" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E19" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D23" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D24" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3445,196 +3589,196 @@
         <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E25" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D26" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E27" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D28" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="E28" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D29" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E29" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E30" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D31" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="E31" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E34" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3647,9 +3791,9 @@
     <hyperlink ref="F4" r:id="rId6" location="isAssociatedWith"/>
     <hyperlink ref="C5" r:id="rId7"/>
     <hyperlink ref="F5" r:id="rId8" location="isAssociatedWith"/>
-    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="C6" r:id="rId9" location="AFR_0001213"/>
     <hyperlink ref="F6" r:id="rId10" location="isAssociatedWith"/>
-    <hyperlink ref="C7" r:id="rId11" location="AFR_0001213"/>
+    <hyperlink ref="C7" r:id="rId11"/>
     <hyperlink ref="F7" r:id="rId12" location="isAssociatedWith"/>
     <hyperlink ref="C8" r:id="rId13"/>
     <hyperlink ref="F8" r:id="rId14" location="isAssociatedWith"/>
@@ -3720,410 +3864,410 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D2">
         <v>3436</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D3">
         <v>3283</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D6">
         <v>2422</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D7">
         <v>2421</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D8">
         <v>3431</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D9">
         <v>3096</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D10" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D11">
         <v>3695</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D12">
         <v>3357</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B13" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D13">
         <v>222</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D14">
         <v>221</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D15" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D16">
         <v>1812</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B17" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D17">
         <v>214</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B18" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C18" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D18">
         <v>148</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D19">
         <v>3081</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D20">
         <v>153</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C21" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D21">
         <v>3802</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D22">
         <v>3359</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C23" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D23">
         <v>3080</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B24" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C24" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D24">
         <v>2428</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -4166,138 +4310,138 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4324,53 +4468,53 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D2">
         <v>500</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D3">
         <v>499</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>